<commit_message>
Setting up inital code
</commit_message>
<xml_diff>
--- a/Palindrome/Palindrome.xlsx
+++ b/Palindrome/Palindrome.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cecfc914.sharepoint.com/sites/Section_76896/Shared Documents/General/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Isaiah\source\repos\Palindrome\Palindrome\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="14_{9FCB01AF-12CD-42E5-B55E-E438F9EF9B5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0C46F4B9-02C7-4483-BE6E-5BEC2A46432C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF68F4EC-0A45-433F-A494-E475141C2C33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11640" xr2:uid="{8BA1E9C4-D659-4A4F-BF92-4DC79AAA710B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{8BA1E9C4-D659-4A4F-BF92-4DC79AAA710B}"/>
   </bookViews>
   <sheets>
     <sheet name="Palendrome" sheetId="1" r:id="rId1"/>
@@ -121,7 +121,7 @@
 Allow user to exit or type another string</t>
   </si>
   <si>
-    <t>&lt;Your Name&gt;</t>
+    <t>Isaiah</t>
   </si>
 </sst>
 </file>
@@ -517,8 +517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{143417AB-3150-4606-8EA9-D3AAD9512135}">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -614,7 +614,7 @@
       </c>
       <c r="C11" t="str">
         <f>$C$6</f>
-        <v>&lt;Your Name&gt;</v>
+        <v>Isaiah</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>14</v>
@@ -632,7 +632,7 @@
       </c>
       <c r="C12" t="str">
         <f>$C$6</f>
-        <v>&lt;Your Name&gt;</v>
+        <v>Isaiah</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>17</v>
@@ -672,7 +672,7 @@
       </c>
       <c r="C15" t="str">
         <f>$C$6</f>
-        <v>&lt;Your Name&gt;</v>
+        <v>Isaiah</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>22</v>
@@ -690,7 +690,7 @@
       </c>
       <c r="C16" t="str">
         <f>$C$6</f>
-        <v>&lt;Your Name&gt;</v>
+        <v>Isaiah</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
Finishing up the check and main funtions
</commit_message>
<xml_diff>
--- a/Palindrome/Palindrome.xlsx
+++ b/Palindrome/Palindrome.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Isaiah\source\repos\Palindrome\Palindrome\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF68F4EC-0A45-433F-A494-E475141C2C33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E2BDCCB-46ED-4FB2-B25E-6B899E6B9B24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{8BA1E9C4-D659-4A4F-BF92-4DC79AAA710B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
   <si>
     <t>Scrum Report for Palindrome Project</t>
   </si>
@@ -75,9 +75,6 @@
   </si>
   <si>
     <t>Status</t>
-  </si>
-  <si>
-    <t>Not started</t>
   </si>
   <si>
     <t>Read string and report if
@@ -122,6 +119,24 @@
   </si>
   <si>
     <t>Isaiah</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>Think of Palindromes that are good tests for your program. Like: Race Car, A Toyota's a Toyota, Do geese see God?</t>
+  </si>
+  <si>
+    <t>complete</t>
+  </si>
+  <si>
+    <t>Reduce takes a value because I want to use it later in the code</t>
+  </si>
+  <si>
+    <t>the check function originally didn't work correctly with even palindromes</t>
+  </si>
+  <si>
+    <t>with my original way of creating the reduce function by removing the specific characters instael of only looking for what characters I wanted, the apostrophies messed up the code that checks for palindromes</t>
   </si>
 </sst>
 </file>
@@ -176,7 +191,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -199,6 +214,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -515,10 +533,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{143417AB-3150-4606-8EA9-D3AAD9512135}">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -571,7 +589,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -591,18 +609,18 @@
         <v>11</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>12</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>9</v>
@@ -617,89 +635,120 @@
         <v>Isaiah</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E11" s="6">
         <v>1</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="G11" s="4"/>
     </row>
     <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C12" t="str">
         <f>$C$6</f>
         <v>Isaiah</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E12" s="6">
         <v>3</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="G12" s="4"/>
+    </row>
+    <row r="13" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="D13" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E13" s="6">
         <v>2</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>13</v>
+        <v>28</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="D14" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E14" s="6">
         <v>2</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="G14" s="4"/>
     </row>
     <row r="15" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C15" t="str">
         <f>$C$6</f>
         <v>Isaiah</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E15" s="6">
         <v>5</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>13</v>
+        <v>28</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C16" t="str">
         <f>$C$6</f>
         <v>Isaiah</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E16" s="6">
         <v>8</v>
       </c>
       <c r="F16" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G16" s="4"/>
+    </row>
+    <row r="17" spans="2:7" ht="180" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" t="str">
+        <f>$C$6</f>
+        <v>Isaiah</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E17" s="6">
         <v>13</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finishing the scrum report
</commit_message>
<xml_diff>
--- a/Palindrome/Palindrome.xlsx
+++ b/Palindrome/Palindrome.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Isaiah\source\repos\Palindrome\Palindrome\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E2BDCCB-46ED-4FB2-B25E-6B899E6B9B24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5801EEC-ECF3-4B46-A7DA-3507CB9E0310}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{8BA1E9C4-D659-4A4F-BF92-4DC79AAA710B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
   <si>
     <t>Scrum Report for Palindrome Project</t>
   </si>
@@ -137,6 +137,12 @@
   </si>
   <si>
     <t>with my original way of creating the reduce function by removing the specific characters instael of only looking for what characters I wanted, the apostrophies messed up the code that checks for palindromes</t>
+  </si>
+  <si>
+    <t>reduce makes all of the letters lowercase to make the check funtion easier to use.</t>
+  </si>
+  <si>
+    <t>the reduce function originally worled differsent than it dos not because I realized that it would be easier to just take the letters and numbers I wanted instead of take out a few that were specified.</t>
   </si>
 </sst>
 </file>
@@ -209,14 +215,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -535,8 +541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{143417AB-3150-4606-8EA9-D3AAD9512135}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -549,16 +555,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
@@ -601,10 +607,10 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="8"/>
+      <c r="C9" s="9"/>
       <c r="D9" s="2" t="s">
         <v>11</v>
       </c>
@@ -645,7 +651,7 @@
       </c>
       <c r="G11" s="4"/>
     </row>
-    <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="165" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
         <v>17</v>
       </c>
@@ -662,7 +668,9 @@
       <c r="F12" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="G12" s="4"/>
+      <c r="G12" s="4" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="13" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="D13" s="4" t="s">
@@ -674,11 +682,11 @@
       <c r="F13" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="G13" s="9" t="s">
+      <c r="G13" s="7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="D14" s="4" t="s">
         <v>19</v>
       </c>
@@ -688,7 +696,9 @@
       <c r="F14" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="G14" s="4"/>
+      <c r="G14" s="4" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="15" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">

</xml_diff>